<commit_message>
feat: add main algorithm
main 함수 알고리즘 작성
</commit_message>
<xml_diff>
--- a/pitcher.xlsx
+++ b/pitcher.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seojaehyeon/Desktop/BigData/finalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1B03A4-042E-F14E-99C0-FF7F5C8EEEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856D9A6E-4949-2847-96D3-AEC8D04FB66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="4860" windowWidth="28100" windowHeight="17380" xr2:uid="{7F93778A-329B-6649-8635-221FB8A1B12C}"/>
+    <workbookView xWindow="5340" yWindow="10600" windowWidth="28100" windowHeight="17380" xr2:uid="{7F93778A-329B-6649-8635-221FB8A1B12C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ERA</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,47 +46,61 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>WHIP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>H</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"직구": 52.3, "슬라이더": 27.1, "커브": 20.6}</t>
-  </si>
-  <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Usage</t>
+    <t>폰세</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>SV</t>
+  </si>
+  <si>
+    <t>HLD</t>
+  </si>
+  <si>
+    <t>WPCT</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>HBP</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>WHIP</t>
   </si>
 </sst>
 </file>
@@ -111,11 +125,10 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
+      <color theme="1"/>
+      <name val="돋움"/>
       <family val="2"/>
       <charset val="129"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,11 +153,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -481,55 +500,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7891BC9C-CC0A-B24E-98A1-3C5F80E6132A}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="J2" s="2">
+        <v>85</v>
+      </c>
+      <c r="K2" s="2">
+        <v>52</v>
+      </c>
+      <c r="L2" s="2">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="L2" s="1" t="s">
-        <v>10</v>
+      <c r="M2" s="2">
+        <v>20</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
+        <v>112</v>
+      </c>
+      <c r="P2" s="2">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>17</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: xlsx inning number fix
</commit_message>
<xml_diff>
--- a/pitcher.xlsx
+++ b/pitcher.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seojaehyeon/Desktop/BigData/finalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA399B0-C9C2-E344-BC6C-398BCFCBB87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8754A4-839F-5D4F-B89A-8DA45F19156C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="1060" windowWidth="16840" windowHeight="21040" xr2:uid="{7F93778A-329B-6649-8635-221FB8A1B12C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="146">
   <si>
     <t>ERA</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,9 +90,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>13 ⅓</t>
-  </si>
-  <si>
     <t>최민준</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -101,9 +98,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>21 ⅓</t>
-  </si>
-  <si>
     <t>조병현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,9 +106,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37 ⅓</t>
-  </si>
-  <si>
     <t>김광현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,9 +114,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>31 ⅔</t>
-  </si>
-  <si>
     <t>이로운</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -138,16 +126,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>29 ⅔</t>
-  </si>
-  <si>
     <t>화이트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>68 ⅔</t>
-  </si>
-  <si>
     <t>배찬승</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -156,9 +138,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>30 ⅓</t>
-  </si>
-  <si>
     <t>최원태</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -171,23 +150,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>103 ⅓</t>
-  </si>
-  <si>
     <t>김재윤</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>30 ⅔</t>
-  </si>
-  <si>
     <t>김태훈</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>35 ⅓</t>
-  </si>
-  <si>
     <t>이호성</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -204,9 +174,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5 ⅓</t>
-  </si>
-  <si>
     <t>원태인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -219,9 +186,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>14 ⅔</t>
-  </si>
-  <si>
     <t>NC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -230,16 +194,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>90 ⅓</t>
-  </si>
-  <si>
     <t>배재환</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>27 ⅔</t>
-  </si>
-  <si>
     <t>최성영</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -248,23 +206,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>31 ⅓</t>
-  </si>
-  <si>
     <t>김진호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8 ⅔</t>
-  </si>
-  <si>
     <t>김영규</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4 ⅓</t>
-  </si>
-  <si>
     <t>이준혁</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -281,23 +230,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>33 ⅔</t>
-  </si>
-  <si>
     <t>신민혁</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>63 ⅓</t>
-  </si>
-  <si>
     <t>라일리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>95 ⅓</t>
-  </si>
-  <si>
     <t>최준용</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -310,9 +250,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>90 ⅔</t>
-  </si>
-  <si>
     <t>감보아</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -325,9 +262,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>38 ⅔</t>
-  </si>
-  <si>
     <t>정현수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -336,30 +270,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>39 ⅓</t>
-  </si>
-  <si>
     <t>김상수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>29 ⅓</t>
-  </si>
-  <si>
     <t>김원중</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>34 ⅔</t>
-  </si>
-  <si>
     <t>이민석</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>35 ⅔</t>
-  </si>
-  <si>
     <t>나균안</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -372,9 +294,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2 ⅔</t>
-  </si>
-  <si>
     <t>치리노스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -387,9 +306,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>86 ⅓</t>
-  </si>
-  <si>
     <t>장현식</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -410,9 +326,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>18 ⅓</t>
-  </si>
-  <si>
     <t>박명근</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -421,16 +334,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>69 ⅓</t>
-  </si>
-  <si>
     <t>송승기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>80 ⅔</t>
-  </si>
-  <si>
     <t>유영찬</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -447,23 +354,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3 ⅓</t>
-  </si>
-  <si>
     <t>쿠에바스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>88 ⅔</t>
-  </si>
-  <si>
     <t>전용주</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7 ⅓</t>
-  </si>
-  <si>
     <t>헤이수스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -480,23 +378,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1 ⅔</t>
-  </si>
-  <si>
     <t>임준형</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4 ⅔</t>
-  </si>
-  <si>
     <t>오원석</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>78 ⅔</t>
-  </si>
-  <si>
     <t>박영현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -505,9 +394,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>77 ⅔</t>
-  </si>
-  <si>
     <t>원상현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -516,9 +402,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>27 ⅓</t>
-  </si>
-  <si>
     <t>알칸타라</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -531,9 +414,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>47 ⅔</t>
-  </si>
-  <si>
     <t>하영민</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -546,9 +426,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>24 ⅓</t>
-  </si>
-  <si>
     <t>김선기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -557,9 +434,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>16 ⅓</t>
-  </si>
-  <si>
     <t>오석주</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -596,23 +470,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>24 ⅔</t>
-  </si>
-  <si>
     <t>전상현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>39 ⅔</t>
-  </si>
-  <si>
     <t>정해영</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>38 ⅓</t>
-  </si>
-  <si>
     <t>김대유</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -621,9 +486,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>80 ⅓</t>
-  </si>
-  <si>
     <t>김현수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -632,9 +494,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>14 ⅓</t>
-  </si>
-  <si>
     <t>이호민</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -663,9 +522,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>34 ⅓</t>
-  </si>
-  <si>
     <t>황준서</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -674,9 +530,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>20 ⅔</t>
-  </si>
-  <si>
     <t>김범수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -685,16 +538,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>28 ⅔</t>
-  </si>
-  <si>
     <t>김기중</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8 ⅓</t>
-  </si>
-  <si>
     <t>김서현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -707,9 +554,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>101 ⅔</t>
-  </si>
-  <si>
     <t>엄상백</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -718,9 +562,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>98 ⅓</t>
-  </si>
-  <si>
     <t>최지강</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -729,23 +570,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>23 ⅓</t>
-  </si>
-  <si>
     <t>최민석</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>21 ⅔</t>
-  </si>
-  <si>
     <t>최승용</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>72 ⅔</t>
-  </si>
-  <si>
     <t>곽빈</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -762,23 +594,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>37 ⅔</t>
-  </si>
-  <si>
     <t>고효준</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>11 ⅓</t>
-  </si>
-  <si>
     <t>이병헌</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6 ⅓</t>
-  </si>
-  <si>
     <t>이영하</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -787,14 +610,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>89 ⅔</t>
-  </si>
-  <si>
     <t>박치국</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>33 ⅓</t>
   </si>
   <si>
     <t>박정수</t>
@@ -1213,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7891BC9C-CC0A-B24E-98A1-3C5F80E6132A}">
   <dimension ref="A1:R130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1294,8 +1111,8 @@
       <c r="D3" s="2">
         <v>1.58</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
+      <c r="E3" s="2">
+        <v>13.3</v>
       </c>
       <c r="F3" s="2">
         <v>8</v>
@@ -1309,7 +1126,7 @@
     </row>
     <row r="4" spans="1:18" ht="19">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -1335,7 +1152,7 @@
     </row>
     <row r="5" spans="1:18" ht="19">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -1346,8 +1163,8 @@
       <c r="D5" s="2">
         <v>1.5</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
+      <c r="E5" s="2">
+        <v>21.3</v>
       </c>
       <c r="F5" s="2">
         <v>22</v>
@@ -1361,7 +1178,7 @@
     </row>
     <row r="6" spans="1:18" ht="19">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -1387,7 +1204,7 @@
     </row>
     <row r="7" spans="1:18" ht="19">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1398,8 +1215,8 @@
       <c r="D7" s="2">
         <v>1.53</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>19</v>
+      <c r="E7" s="2">
+        <v>37.299999999999997</v>
       </c>
       <c r="F7" s="2">
         <v>38</v>
@@ -1413,7 +1230,7 @@
     </row>
     <row r="8" spans="1:18" ht="19">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -1439,7 +1256,7 @@
     </row>
     <row r="9" spans="1:18" ht="19">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -1450,8 +1267,8 @@
       <c r="D9" s="2">
         <v>1.55</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>22</v>
+      <c r="E9" s="2">
+        <v>31.6</v>
       </c>
       <c r="F9" s="2">
         <v>31</v>
@@ -1465,7 +1282,7 @@
     </row>
     <row r="10" spans="1:18" ht="19">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1491,7 +1308,7 @@
     </row>
     <row r="11" spans="1:18" ht="19">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1517,7 +1334,7 @@
     </row>
     <row r="12" spans="1:18" ht="19">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -1528,8 +1345,8 @@
       <c r="D12" s="2">
         <v>1.45</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>26</v>
+      <c r="E12" s="2">
+        <v>29.6</v>
       </c>
       <c r="F12" s="2">
         <v>21</v>
@@ -1543,7 +1360,7 @@
     </row>
     <row r="13" spans="1:18" ht="19">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -1554,8 +1371,8 @@
       <c r="D13" s="2">
         <v>1.1100000000000001</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>28</v>
+      <c r="E13" s="2">
+        <v>68.599999999999994</v>
       </c>
       <c r="F13" s="2">
         <v>69</v>
@@ -1569,10 +1386,10 @@
     </row>
     <row r="14" spans="1:18" ht="19">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2">
         <v>4.45</v>
@@ -1580,8 +1397,8 @@
       <c r="D14" s="2">
         <v>1.75</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>31</v>
+      <c r="E14" s="2">
+        <v>30.3</v>
       </c>
       <c r="F14" s="2">
         <v>30</v>
@@ -1595,10 +1412,10 @@
     </row>
     <row r="15" spans="1:18" ht="19">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2">
         <v>5.18</v>
@@ -1621,10 +1438,10 @@
     </row>
     <row r="16" spans="1:18" ht="19">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C16" s="2">
         <v>7</v>
@@ -1647,10 +1464,10 @@
     </row>
     <row r="17" spans="1:9" ht="19">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2">
         <v>2.87</v>
@@ -1658,8 +1475,8 @@
       <c r="D17" s="2">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>35</v>
+      <c r="E17" s="2">
+        <v>103.3</v>
       </c>
       <c r="F17" s="2">
         <v>81</v>
@@ -1673,10 +1490,10 @@
     </row>
     <row r="18" spans="1:9" ht="19">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C18" s="2">
         <v>6.46</v>
@@ -1684,8 +1501,8 @@
       <c r="D18" s="2">
         <v>1.24</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>37</v>
+      <c r="E18" s="2">
+        <v>30.6</v>
       </c>
       <c r="F18" s="2">
         <v>24</v>
@@ -1699,10 +1516,10 @@
     </row>
     <row r="19" spans="1:9" ht="19">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2">
         <v>3.06</v>
@@ -1710,8 +1527,8 @@
       <c r="D19" s="2">
         <v>1.3</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>39</v>
+      <c r="E19" s="2">
+        <v>35.299999999999997</v>
       </c>
       <c r="F19" s="2">
         <v>40</v>
@@ -1725,10 +1542,10 @@
     </row>
     <row r="20" spans="1:9" ht="19">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2">
         <v>5.14</v>
@@ -1751,10 +1568,10 @@
     </row>
     <row r="21" spans="1:9" ht="19">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C21" s="2">
         <v>4.88</v>
@@ -1778,10 +1595,10 @@
     </row>
     <row r="22" spans="1:9" ht="19">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2">
         <v>5</v>
@@ -1805,10 +1622,10 @@
     </row>
     <row r="23" spans="1:9" ht="19">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2">
         <v>3.38</v>
@@ -1816,8 +1633,8 @@
       <c r="D23" s="2">
         <v>1.88</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>44</v>
+      <c r="E23" s="2">
+        <v>5.3</v>
       </c>
       <c r="F23" s="2">
         <v>4</v>
@@ -1832,10 +1649,10 @@
     </row>
     <row r="24" spans="1:9" ht="19">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C24" s="2">
         <v>2.59</v>
@@ -1859,10 +1676,10 @@
     </row>
     <row r="25" spans="1:9" ht="19">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C25" s="2">
         <v>5.85</v>
@@ -1886,10 +1703,10 @@
     </row>
     <row r="26" spans="1:9" ht="19">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C26" s="2">
         <v>1.23</v>
@@ -1897,8 +1714,8 @@
       <c r="D26" s="2">
         <v>0.89</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>48</v>
+      <c r="E26" s="2">
+        <v>14.6</v>
       </c>
       <c r="F26" s="2">
         <v>9</v>
@@ -1913,10 +1730,10 @@
     </row>
     <row r="27" spans="1:9" ht="19">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C27" s="2">
         <v>3.29</v>
@@ -1924,8 +1741,8 @@
       <c r="D27" s="2">
         <v>1.38</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>51</v>
+      <c r="E27" s="2">
+        <v>90.3</v>
       </c>
       <c r="F27" s="2">
         <v>70</v>
@@ -1940,10 +1757,10 @@
     </row>
     <row r="28" spans="1:9" ht="19">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C28" s="2">
         <v>3.58</v>
@@ -1951,8 +1768,8 @@
       <c r="D28" s="2">
         <v>1.23</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>53</v>
+      <c r="E28" s="2">
+        <v>27.6</v>
       </c>
       <c r="F28" s="2">
         <v>26</v>
@@ -1967,10 +1784,10 @@
     </row>
     <row r="29" spans="1:9" ht="19">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C29" s="2">
         <v>5.34</v>
@@ -1978,8 +1795,8 @@
       <c r="D29" s="2">
         <v>1.71</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>31</v>
+      <c r="E29" s="2">
+        <v>30.3</v>
       </c>
       <c r="F29" s="2">
         <v>20</v>
@@ -1994,10 +1811,10 @@
     </row>
     <row r="30" spans="1:9" ht="19">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C30" s="2">
         <v>6.32</v>
@@ -2005,8 +1822,8 @@
       <c r="D30" s="2">
         <v>1.72</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>56</v>
+      <c r="E30" s="2">
+        <v>31.3</v>
       </c>
       <c r="F30" s="2">
         <v>17</v>
@@ -2021,10 +1838,10 @@
     </row>
     <row r="31" spans="1:9" ht="19">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C31" s="2">
         <v>2.97</v>
@@ -2032,8 +1849,8 @@
       <c r="D31" s="2">
         <v>1.19</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>31</v>
+      <c r="E31" s="2">
+        <v>30.3</v>
       </c>
       <c r="F31" s="2">
         <v>28</v>
@@ -2048,10 +1865,10 @@
     </row>
     <row r="32" spans="1:9" ht="19">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C32" s="2">
         <v>4.1500000000000004</v>
@@ -2059,8 +1876,8 @@
       <c r="D32" s="2">
         <v>1.62</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>58</v>
+      <c r="E32" s="2">
+        <v>8.6</v>
       </c>
       <c r="F32" s="2">
         <v>5</v>
@@ -2075,10 +1892,10 @@
     </row>
     <row r="33" spans="1:9" ht="19">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
@@ -2086,8 +1903,8 @@
       <c r="D33" s="2">
         <v>0.46</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>60</v>
+      <c r="E33" s="2">
+        <v>4.3</v>
       </c>
       <c r="F33" s="2">
         <v>3</v>
@@ -2102,10 +1919,10 @@
     </row>
     <row r="34" spans="1:9" ht="19">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C34" s="2">
         <v>8.25</v>
@@ -2129,10 +1946,10 @@
     </row>
     <row r="35" spans="1:9" ht="19">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C35" s="2">
         <v>2.57</v>
@@ -2156,10 +1973,10 @@
     </row>
     <row r="36" spans="1:9" ht="19">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C36" s="2">
         <v>6.23</v>
@@ -2183,10 +2000,10 @@
     </row>
     <row r="37" spans="1:9" ht="19">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C37" s="2">
         <v>4.01</v>
@@ -2194,8 +2011,8 @@
       <c r="D37" s="2">
         <v>1.22</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>65</v>
+      <c r="E37" s="2">
+        <v>33.6</v>
       </c>
       <c r="F37" s="2">
         <v>28</v>
@@ -2210,10 +2027,10 @@
     </row>
     <row r="38" spans="1:9" ht="19">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C38" s="2">
         <v>3.84</v>
@@ -2221,8 +2038,8 @@
       <c r="D38" s="2">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>67</v>
+      <c r="E38" s="2">
+        <v>63.3</v>
       </c>
       <c r="F38" s="2">
         <v>39</v>
@@ -2237,10 +2054,10 @@
     </row>
     <row r="39" spans="1:9" ht="19">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C39" s="2">
         <v>3.02</v>
@@ -2248,8 +2065,8 @@
       <c r="D39" s="2">
         <v>1.07</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>69</v>
+      <c r="E39" s="2">
+        <v>95.3</v>
       </c>
       <c r="F39" s="2">
         <v>123</v>
@@ -2264,10 +2081,10 @@
     </row>
     <row r="40" spans="1:9" ht="19">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C40" s="2">
         <v>3</v>
@@ -2291,10 +2108,10 @@
     </row>
     <row r="41" spans="1:9" ht="19">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C41" s="2">
         <v>3.67</v>
@@ -2302,8 +2119,8 @@
       <c r="D41" s="2">
         <v>1.39</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>73</v>
+      <c r="E41" s="2">
+        <v>90.6</v>
       </c>
       <c r="F41" s="2">
         <v>89</v>
@@ -2318,10 +2135,10 @@
     </row>
     <row r="42" spans="1:9" ht="19">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C42" s="2">
         <v>2.37</v>
@@ -2329,8 +2146,8 @@
       <c r="D42" s="2">
         <v>1.02</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>31</v>
+      <c r="E42" s="2">
+        <v>30.3</v>
       </c>
       <c r="F42" s="2">
         <v>34</v>
@@ -2345,10 +2162,10 @@
     </row>
     <row r="43" spans="1:9" ht="19">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -2372,10 +2189,10 @@
     </row>
     <row r="44" spans="1:9" ht="19">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C44" s="2">
         <v>4.1900000000000004</v>
@@ -2383,8 +2200,8 @@
       <c r="D44" s="2">
         <v>1.32</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>77</v>
+      <c r="E44" s="2">
+        <v>38.6</v>
       </c>
       <c r="F44" s="2">
         <v>31</v>
@@ -2399,10 +2216,10 @@
     </row>
     <row r="45" spans="1:9" ht="19">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C45" s="2">
         <v>2.79</v>
@@ -2426,10 +2243,10 @@
     </row>
     <row r="46" spans="1:9" ht="19">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C46" s="2">
         <v>3.66</v>
@@ -2437,8 +2254,8 @@
       <c r="D46" s="2">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>80</v>
+      <c r="E46" s="2">
+        <v>39.299999999999997</v>
       </c>
       <c r="F46" s="2">
         <v>25</v>
@@ -2453,10 +2270,10 @@
     </row>
     <row r="47" spans="1:9" ht="19">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C47" s="2">
         <v>5.83</v>
@@ -2464,8 +2281,8 @@
       <c r="D47" s="2">
         <v>1.67</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>82</v>
+      <c r="E47" s="2">
+        <v>29.3</v>
       </c>
       <c r="F47" s="2">
         <v>24</v>
@@ -2480,10 +2297,10 @@
     </row>
     <row r="48" spans="1:9" ht="19">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C48" s="2">
         <v>1.56</v>
@@ -2491,8 +2308,8 @@
       <c r="D48" s="2">
         <v>1.21</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>84</v>
+      <c r="E48" s="2">
+        <v>34.6</v>
       </c>
       <c r="F48" s="2">
         <v>40</v>
@@ -2507,10 +2324,10 @@
     </row>
     <row r="49" spans="1:9" ht="19">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C49" s="2">
         <v>5.05</v>
@@ -2518,8 +2335,8 @@
       <c r="D49" s="2">
         <v>1.49</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>86</v>
+      <c r="E49" s="2">
+        <v>35.6</v>
       </c>
       <c r="F49" s="2">
         <v>26</v>
@@ -2534,10 +2351,10 @@
     </row>
     <row r="50" spans="1:9" ht="19">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C50" s="2">
         <v>4.46</v>
@@ -2545,8 +2362,8 @@
       <c r="D50" s="2">
         <v>1.6</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>28</v>
+      <c r="E50" s="2">
+        <v>68.599999999999994</v>
       </c>
       <c r="F50" s="2">
         <v>49</v>
@@ -2561,10 +2378,10 @@
     </row>
     <row r="51" spans="1:9" ht="19">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C51" s="2">
         <v>4.8099999999999996</v>
@@ -2588,10 +2405,10 @@
     </row>
     <row r="52" spans="1:9" ht="19">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C52" s="2">
         <v>30.38</v>
@@ -2599,8 +2416,8 @@
       <c r="D52" s="2">
         <v>4.13</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>90</v>
+      <c r="E52" s="2">
+        <v>2.6</v>
       </c>
       <c r="F52" s="2">
         <v>4</v>
@@ -2615,10 +2432,10 @@
     </row>
     <row r="53" spans="1:9" ht="19">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C53" s="2">
         <v>3.21</v>
@@ -2626,8 +2443,8 @@
       <c r="D53" s="2">
         <v>1.21</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>69</v>
+      <c r="E53" s="2">
+        <v>95.3</v>
       </c>
       <c r="F53" s="2">
         <v>85</v>
@@ -2642,10 +2459,10 @@
     </row>
     <row r="54" spans="1:9" ht="19">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C54" s="2">
         <v>4.6100000000000003</v>
@@ -2669,10 +2486,10 @@
     </row>
     <row r="55" spans="1:9" ht="19">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C55" s="2">
         <v>2.61</v>
@@ -2680,8 +2497,8 @@
       <c r="D55" s="2">
         <v>1.18</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>94</v>
+      <c r="E55" s="2">
+        <v>86.3</v>
       </c>
       <c r="F55" s="2">
         <v>59</v>
@@ -2696,10 +2513,10 @@
     </row>
     <row r="56" spans="1:9" ht="19">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C56" s="2">
         <v>2.4500000000000002</v>
@@ -2723,10 +2540,10 @@
     </row>
     <row r="57" spans="1:9" ht="19">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C57" s="2">
         <v>3.49</v>
@@ -2734,8 +2551,8 @@
       <c r="D57" s="2">
         <v>1.24</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>77</v>
+      <c r="E57" s="2">
+        <v>38.6</v>
       </c>
       <c r="F57" s="2">
         <v>33</v>
@@ -2750,10 +2567,10 @@
     </row>
     <row r="58" spans="1:9" ht="19">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B58" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C58" s="2">
         <v>2.9</v>
@@ -2777,10 +2594,10 @@
     </row>
     <row r="59" spans="1:9" ht="19">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C59" s="2">
         <v>4.4000000000000004</v>
@@ -2788,8 +2605,8 @@
       <c r="D59" s="2">
         <v>1.43</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>37</v>
+      <c r="E59" s="2">
+        <v>30.6</v>
       </c>
       <c r="F59" s="2">
         <v>26</v>
@@ -2804,10 +2621,10 @@
     </row>
     <row r="60" spans="1:9" ht="19">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C60" s="2">
         <v>1.96</v>
@@ -2815,8 +2632,8 @@
       <c r="D60" s="2">
         <v>1.31</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>100</v>
+      <c r="E60" s="2">
+        <v>18.3</v>
       </c>
       <c r="F60" s="2">
         <v>19</v>
@@ -2831,10 +2648,10 @@
     </row>
     <row r="61" spans="1:9" ht="19">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C61" s="2">
         <v>3.98</v>
@@ -2842,8 +2659,8 @@
       <c r="D61" s="2">
         <v>1.23</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>22</v>
+      <c r="E61" s="2">
+        <v>31.6</v>
       </c>
       <c r="F61" s="2">
         <v>26</v>
@@ -2858,10 +2675,10 @@
     </row>
     <row r="62" spans="1:9" ht="19">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C62" s="2">
         <v>4.54</v>
@@ -2869,8 +2686,8 @@
       <c r="D62" s="2">
         <v>1.4</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>103</v>
+      <c r="E62" s="2">
+        <v>69.3</v>
       </c>
       <c r="F62" s="2">
         <v>66</v>
@@ -2885,10 +2702,10 @@
     </row>
     <row r="63" spans="1:9" ht="19">
       <c r="A63" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C63" s="2">
         <v>2.57</v>
@@ -2896,8 +2713,8 @@
       <c r="D63" s="2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>105</v>
+      <c r="E63" s="2">
+        <v>80.599999999999994</v>
       </c>
       <c r="F63" s="2">
         <v>73</v>
@@ -2912,10 +2729,10 @@
     </row>
     <row r="64" spans="1:9" ht="19">
       <c r="A64" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C64" s="2">
         <v>2.57</v>
@@ -2939,10 +2756,10 @@
     </row>
     <row r="65" spans="1:9" ht="19">
       <c r="A65" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C65" s="2">
         <v>5.4</v>
@@ -2950,8 +2767,8 @@
       <c r="D65" s="2">
         <v>0.9</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>110</v>
+      <c r="E65" s="2">
+        <v>3.3</v>
       </c>
       <c r="F65" s="2">
         <v>4</v>
@@ -2966,10 +2783,10 @@
     </row>
     <row r="66" spans="1:9" ht="19">
       <c r="A66" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B66" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C66" s="2">
         <v>5.38</v>
@@ -2977,8 +2794,8 @@
       <c r="D66" s="2">
         <v>1.49</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>112</v>
+      <c r="E66" s="2">
+        <v>88.6</v>
       </c>
       <c r="F66" s="2">
         <v>56</v>
@@ -2993,10 +2810,10 @@
     </row>
     <row r="67" spans="1:9" ht="19">
       <c r="A67" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C67" s="2">
         <v>2.4500000000000002</v>
@@ -3004,8 +2821,8 @@
       <c r="D67" s="2">
         <v>1.91</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>114</v>
+      <c r="E67" s="2">
+        <v>7.3</v>
       </c>
       <c r="F67" s="2">
         <v>5</v>
@@ -3020,10 +2837,10 @@
     </row>
     <row r="68" spans="1:9" ht="19">
       <c r="A68" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B68" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C68" s="2">
         <v>2.75</v>
@@ -3047,10 +2864,10 @@
     </row>
     <row r="69" spans="1:9" ht="19">
       <c r="A69" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C69" s="2">
         <v>2.57</v>
@@ -3074,10 +2891,10 @@
     </row>
     <row r="70" spans="1:9" ht="19">
       <c r="A70" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="B70" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C70" s="2">
         <v>2.92</v>
@@ -3101,10 +2918,10 @@
     </row>
     <row r="71" spans="1:9" ht="19">
       <c r="A71" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C71" s="2">
         <v>5.4</v>
@@ -3112,8 +2929,8 @@
       <c r="D71" s="2">
         <v>1.8</v>
       </c>
-      <c r="E71" s="2" t="s">
-        <v>119</v>
+      <c r="E71" s="2">
+        <v>1.6</v>
       </c>
       <c r="F71" s="2">
         <v>1</v>
@@ -3128,10 +2945,10 @@
     </row>
     <row r="72" spans="1:9" ht="19">
       <c r="A72" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="B72" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C72" s="2">
         <v>1.93</v>
@@ -3139,8 +2956,8 @@
       <c r="D72" s="2">
         <v>1.29</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>121</v>
+      <c r="E72" s="2">
+        <v>4.5999999999999996</v>
       </c>
       <c r="F72" s="2">
         <v>2</v>
@@ -3155,10 +2972,10 @@
     </row>
     <row r="73" spans="1:9" ht="19">
       <c r="A73" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="B73" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C73" s="2">
         <v>3.09</v>
@@ -3166,8 +2983,8 @@
       <c r="D73" s="2">
         <v>1.27</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>123</v>
+      <c r="E73" s="2">
+        <v>78.599999999999994</v>
       </c>
       <c r="F73" s="2">
         <v>70</v>
@@ -3182,10 +2999,10 @@
     </row>
     <row r="74" spans="1:9" ht="19">
       <c r="A74" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="B74" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C74" s="2">
         <v>2.54</v>
@@ -3209,10 +3026,10 @@
     </row>
     <row r="75" spans="1:9" ht="19">
       <c r="A75" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="B75" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C75" s="2">
         <v>3.13</v>
@@ -3220,8 +3037,8 @@
       <c r="D75" s="2">
         <v>1.18</v>
       </c>
-      <c r="E75" s="2" t="s">
-        <v>126</v>
+      <c r="E75" s="2">
+        <v>77.599999999999994</v>
       </c>
       <c r="F75" s="2">
         <v>78</v>
@@ -3236,10 +3053,10 @@
     </row>
     <row r="76" spans="1:9" ht="19">
       <c r="A76" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="B76" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C76" s="2">
         <v>3.25</v>
@@ -3263,10 +3080,10 @@
     </row>
     <row r="77" spans="1:9" ht="19">
       <c r="A77" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="B77" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C77" s="2">
         <v>2.63</v>
@@ -3274,8 +3091,8 @@
       <c r="D77" s="2">
         <v>1.02</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>129</v>
+      <c r="E77" s="2">
+        <v>27.3</v>
       </c>
       <c r="F77" s="2">
         <v>16</v>
@@ -3290,10 +3107,10 @@
     </row>
     <row r="78" spans="1:9" ht="19">
       <c r="A78" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="B78" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C78" s="2">
         <v>3.75</v>
@@ -3317,10 +3134,10 @@
     </row>
     <row r="79" spans="1:9" ht="19">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C79" s="2">
         <v>6.04</v>
@@ -3328,8 +3145,8 @@
       <c r="D79" s="2">
         <v>1.49</v>
       </c>
-      <c r="E79" s="2" t="s">
-        <v>133</v>
+      <c r="E79" s="2">
+        <v>47.6</v>
       </c>
       <c r="F79" s="2">
         <v>29</v>
@@ -3344,10 +3161,10 @@
     </row>
     <row r="80" spans="1:9" ht="19">
       <c r="A80" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="B80" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C80" s="2">
         <v>4.88</v>
@@ -3371,10 +3188,10 @@
     </row>
     <row r="81" spans="1:9" ht="19">
       <c r="A81" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="B81" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C81" s="2">
         <v>2.4500000000000002</v>
@@ -3382,8 +3199,8 @@
       <c r="D81" s="2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>82</v>
+      <c r="E81" s="2">
+        <v>29.3</v>
       </c>
       <c r="F81" s="2">
         <v>22</v>
@@ -3398,10 +3215,10 @@
     </row>
     <row r="82" spans="1:9" ht="19">
       <c r="A82" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="B82" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C82" s="2">
         <v>3.33</v>
@@ -3409,8 +3226,8 @@
       <c r="D82" s="2">
         <v>1.68</v>
       </c>
-      <c r="E82" s="2" t="s">
-        <v>137</v>
+      <c r="E82" s="2">
+        <v>24.3</v>
       </c>
       <c r="F82" s="2">
         <v>17</v>
@@ -3425,10 +3242,10 @@
     </row>
     <row r="83" spans="1:9" ht="19">
       <c r="A83" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C83" s="2">
         <v>5.47</v>
@@ -3452,10 +3269,10 @@
     </row>
     <row r="84" spans="1:9" ht="19">
       <c r="A84" t="s">
-        <v>139</v>
+        <v>98</v>
       </c>
       <c r="B84" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C84" s="2">
         <v>6.06</v>
@@ -3463,8 +3280,8 @@
       <c r="D84" s="2">
         <v>1.78</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>140</v>
+      <c r="E84" s="2">
+        <v>16.3</v>
       </c>
       <c r="F84" s="2">
         <v>15</v>
@@ -3479,10 +3296,10 @@
     </row>
     <row r="85" spans="1:9" ht="19">
       <c r="A85" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="B85" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C85" s="2">
         <v>6</v>
@@ -3506,10 +3323,10 @@
     </row>
     <row r="86" spans="1:9" ht="19">
       <c r="A86" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
       <c r="B86" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C86" s="2">
         <v>3</v>
@@ -3531,10 +3348,10 @@
     </row>
     <row r="87" spans="1:9" ht="19">
       <c r="A87" t="s">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="B87" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C87" s="2">
         <v>4.07</v>
@@ -3542,8 +3359,8 @@
       <c r="D87" s="2">
         <v>1.4</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>137</v>
+      <c r="E87" s="2">
+        <v>24.3</v>
       </c>
       <c r="F87" s="2">
         <v>20</v>
@@ -3558,10 +3375,10 @@
     </row>
     <row r="88" spans="1:9" ht="19">
       <c r="A88" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="B88" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C88" s="2">
         <v>3</v>
@@ -3585,10 +3402,10 @@
     </row>
     <row r="89" spans="1:9" ht="19">
       <c r="A89" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="B89" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C89" s="2">
         <v>5.28</v>
@@ -3612,10 +3429,10 @@
     </row>
     <row r="90" spans="1:9" ht="19">
       <c r="A90" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="B90" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C90" s="2">
         <v>16.5</v>
@@ -3639,10 +3456,10 @@
     </row>
     <row r="91" spans="1:9" ht="19">
       <c r="A91" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="B91" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C91" s="2">
         <v>3.63</v>
@@ -3650,8 +3467,8 @@
       <c r="D91" s="2">
         <v>1.59</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>84</v>
+      <c r="E91" s="2">
+        <v>34.6</v>
       </c>
       <c r="F91" s="2">
         <v>36</v>
@@ -3666,10 +3483,10 @@
     </row>
     <row r="92" spans="1:9" ht="19">
       <c r="A92" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="B92" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C92" s="2">
         <v>6.57</v>
@@ -3677,8 +3494,8 @@
       <c r="D92" s="2">
         <v>1.86</v>
       </c>
-      <c r="E92" s="2" t="s">
-        <v>150</v>
+      <c r="E92" s="2">
+        <v>24.6</v>
       </c>
       <c r="F92" s="2">
         <v>23</v>
@@ -3693,10 +3510,10 @@
     </row>
     <row r="93" spans="1:9" ht="19">
       <c r="A93" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="B93" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C93" s="2">
         <v>3.63</v>
@@ -3704,8 +3521,8 @@
       <c r="D93" s="2">
         <v>1.26</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>152</v>
+      <c r="E93" s="2">
+        <v>39.6</v>
       </c>
       <c r="F93" s="2">
         <v>24</v>
@@ -3720,10 +3537,10 @@
     </row>
     <row r="94" spans="1:9" ht="19">
       <c r="A94" t="s">
-        <v>153</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C94" s="2">
         <v>3.29</v>
@@ -3731,8 +3548,8 @@
       <c r="D94" s="2">
         <v>1.43</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>154</v>
+      <c r="E94" s="2">
+        <v>38.299999999999997</v>
       </c>
       <c r="F94" s="2">
         <v>46</v>
@@ -3747,10 +3564,10 @@
     </row>
     <row r="95" spans="1:9" ht="19">
       <c r="A95" t="s">
-        <v>155</v>
+        <v>110</v>
       </c>
       <c r="B95" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C95" s="2">
         <v>32.4</v>
@@ -3758,8 +3575,8 @@
       <c r="D95" s="2">
         <v>3.6</v>
       </c>
-      <c r="E95" s="2" t="s">
-        <v>119</v>
+      <c r="E95" s="2">
+        <v>1.6</v>
       </c>
       <c r="F95" s="2">
         <v>1</v>
@@ -3774,10 +3591,10 @@
     </row>
     <row r="96" spans="1:9" ht="19">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>111</v>
       </c>
       <c r="B96" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C96" s="2">
         <v>3.02</v>
@@ -3785,8 +3602,8 @@
       <c r="D96" s="2">
         <v>1.32</v>
       </c>
-      <c r="E96" s="2" t="s">
-        <v>157</v>
+      <c r="E96" s="2">
+        <v>80.3</v>
       </c>
       <c r="F96" s="2">
         <v>53</v>
@@ -3801,10 +3618,10 @@
     </row>
     <row r="97" spans="1:9" ht="19">
       <c r="A97" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="B97" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C97" s="2">
         <v>2.4500000000000002</v>
@@ -3812,8 +3629,8 @@
       <c r="D97" s="2">
         <v>1.64</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>114</v>
+      <c r="E97" s="2">
+        <v>7.3</v>
       </c>
       <c r="F97" s="2">
         <v>6</v>
@@ -3828,10 +3645,10 @@
     </row>
     <row r="98" spans="1:9" ht="19">
       <c r="A98" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="B98" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C98" s="2">
         <v>7.53</v>
@@ -3839,8 +3656,8 @@
       <c r="D98" s="2">
         <v>1.88</v>
       </c>
-      <c r="E98" s="2" t="s">
-        <v>160</v>
+      <c r="E98" s="2">
+        <v>14.3</v>
       </c>
       <c r="F98" s="2">
         <v>11</v>
@@ -3855,10 +3672,10 @@
     </row>
     <row r="99" spans="1:9" ht="19">
       <c r="A99" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="B99" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C99" s="2">
         <v>2.7</v>
@@ -3866,8 +3683,8 @@
       <c r="D99" s="2">
         <v>1.5</v>
       </c>
-      <c r="E99" s="2" t="s">
-        <v>110</v>
+      <c r="E99" s="2">
+        <v>3.3</v>
       </c>
       <c r="F99" s="2">
         <v>1</v>
@@ -3882,10 +3699,10 @@
     </row>
     <row r="100" spans="1:9" ht="19">
       <c r="A100" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
       <c r="B100" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C100" s="2">
         <v>3.03</v>
@@ -3909,10 +3726,10 @@
     </row>
     <row r="101" spans="1:9" ht="19">
       <c r="A101" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="B101" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C101" s="2">
         <v>0.5</v>
@@ -3936,10 +3753,10 @@
     </row>
     <row r="102" spans="1:9" ht="19">
       <c r="A102" t="s">
-        <v>164</v>
+        <v>117</v>
       </c>
       <c r="B102" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C102" s="2">
         <v>5.0999999999999996</v>
@@ -3947,8 +3764,8 @@
       <c r="D102" s="2">
         <v>1.55</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>126</v>
+      <c r="E102" s="2">
+        <v>77.599999999999994</v>
       </c>
       <c r="F102" s="2">
         <v>62</v>
@@ -3963,10 +3780,10 @@
     </row>
     <row r="103" spans="1:9" ht="19">
       <c r="A103" t="s">
-        <v>165</v>
+        <v>118</v>
       </c>
       <c r="B103" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="C103" s="2">
         <v>5.86</v>
@@ -3990,7 +3807,7 @@
     </row>
     <row r="104" spans="1:9" ht="19">
       <c r="A104" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
       <c r="B104" t="s">
         <v>4</v>
@@ -4016,7 +3833,7 @@
     </row>
     <row r="105" spans="1:9" ht="19">
       <c r="A105" t="s">
-        <v>167</v>
+        <v>120</v>
       </c>
       <c r="B105" t="s">
         <v>4</v>
@@ -4027,8 +3844,8 @@
       <c r="D105" s="2">
         <v>1.22</v>
       </c>
-      <c r="E105" s="2" t="s">
-        <v>168</v>
+      <c r="E105" s="2">
+        <v>34.299999999999997</v>
       </c>
       <c r="F105" s="2">
         <v>27</v>
@@ -4042,7 +3859,7 @@
     </row>
     <row r="106" spans="1:9" ht="19">
       <c r="A106" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="B106" t="s">
         <v>4</v>
@@ -4053,8 +3870,8 @@
       <c r="D106" s="2">
         <v>1.27</v>
       </c>
-      <c r="E106" s="2" t="s">
-        <v>137</v>
+      <c r="E106" s="2">
+        <v>24.3</v>
       </c>
       <c r="F106" s="2">
         <v>22</v>
@@ -4068,7 +3885,7 @@
     </row>
     <row r="107" spans="1:9" ht="19">
       <c r="A107" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="B107" t="s">
         <v>4</v>
@@ -4079,8 +3896,8 @@
       <c r="D107" s="2">
         <v>1.45</v>
       </c>
-      <c r="E107" s="2" t="s">
-        <v>171</v>
+      <c r="E107" s="2">
+        <v>20.6</v>
       </c>
       <c r="F107" s="2">
         <v>21</v>
@@ -4094,7 +3911,7 @@
     </row>
     <row r="108" spans="1:9" ht="19">
       <c r="A108" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
       <c r="B108" t="s">
         <v>4</v>
@@ -4120,7 +3937,7 @@
     </row>
     <row r="109" spans="1:9" ht="19">
       <c r="A109" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="B109" t="s">
         <v>4</v>
@@ -4131,8 +3948,8 @@
       <c r="D109" s="2">
         <v>1.6</v>
       </c>
-      <c r="E109" s="2" t="s">
-        <v>174</v>
+      <c r="E109" s="2">
+        <v>28.6</v>
       </c>
       <c r="F109" s="2">
         <v>25</v>
@@ -4146,7 +3963,7 @@
     </row>
     <row r="110" spans="1:9" ht="19">
       <c r="A110" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="B110" t="s">
         <v>4</v>
@@ -4157,8 +3974,8 @@
       <c r="D110" s="2">
         <v>0.96</v>
       </c>
-      <c r="E110" s="2" t="s">
-        <v>176</v>
+      <c r="E110" s="2">
+        <v>8.3000000000000007</v>
       </c>
       <c r="F110" s="2">
         <v>4</v>
@@ -4172,7 +3989,7 @@
     </row>
     <row r="111" spans="1:9" ht="19">
       <c r="A111" t="s">
-        <v>177</v>
+        <v>126</v>
       </c>
       <c r="B111" t="s">
         <v>4</v>
@@ -4183,8 +4000,8 @@
       <c r="D111" s="2">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E111" s="2" t="s">
-        <v>86</v>
+      <c r="E111" s="2">
+        <v>35.6</v>
       </c>
       <c r="F111" s="2">
         <v>40</v>
@@ -4198,7 +4015,7 @@
     </row>
     <row r="112" spans="1:9" ht="19">
       <c r="A112" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
       <c r="B112" t="s">
         <v>4</v>
@@ -4224,7 +4041,7 @@
     </row>
     <row r="113" spans="1:9" ht="19">
       <c r="A113" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="B113" t="s">
         <v>4</v>
@@ -4261,8 +4078,8 @@
       <c r="D114" s="2">
         <v>0.85</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>180</v>
+      <c r="E114" s="2">
+        <v>101.6</v>
       </c>
       <c r="F114" s="2">
         <v>141</v>
@@ -4276,7 +4093,7 @@
     </row>
     <row r="115" spans="1:9" ht="19">
       <c r="A115" t="s">
-        <v>181</v>
+        <v>129</v>
       </c>
       <c r="B115" t="s">
         <v>4</v>
@@ -4303,7 +4120,7 @@
     </row>
     <row r="116" spans="1:9" ht="19">
       <c r="A116" t="s">
-        <v>182</v>
+        <v>130</v>
       </c>
       <c r="B116" t="s">
         <v>4</v>
@@ -4314,8 +4131,8 @@
       <c r="D116" s="2">
         <v>1</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>183</v>
+      <c r="E116" s="2">
+        <v>98.3</v>
       </c>
       <c r="F116" s="2">
         <v>110</v>
@@ -4329,10 +4146,10 @@
     </row>
     <row r="117" spans="1:9" ht="19">
       <c r="A117" t="s">
-        <v>184</v>
+        <v>131</v>
       </c>
       <c r="B117" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C117" s="2">
         <v>5.4</v>
@@ -4340,8 +4157,8 @@
       <c r="D117" s="2">
         <v>1.63</v>
       </c>
-      <c r="E117" s="2" t="s">
-        <v>186</v>
+      <c r="E117" s="2">
+        <v>23.3</v>
       </c>
       <c r="F117" s="2">
         <v>29</v>
@@ -4356,10 +4173,10 @@
     </row>
     <row r="118" spans="1:9" ht="19">
       <c r="A118" t="s">
-        <v>187</v>
+        <v>133</v>
       </c>
       <c r="B118" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C118" s="2">
         <v>3.32</v>
@@ -4367,8 +4184,8 @@
       <c r="D118" s="2">
         <v>1.29</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>188</v>
+      <c r="E118" s="2">
+        <v>21.6</v>
       </c>
       <c r="F118" s="2">
         <v>12</v>
@@ -4382,10 +4199,10 @@
     </row>
     <row r="119" spans="1:9" ht="19">
       <c r="A119" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
       <c r="B119" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C119" s="2">
         <v>4.83</v>
@@ -4393,8 +4210,8 @@
       <c r="D119" s="2">
         <v>1.42</v>
       </c>
-      <c r="E119" s="2" t="s">
-        <v>190</v>
+      <c r="E119" s="2">
+        <v>72.599999999999994</v>
       </c>
       <c r="F119" s="2">
         <v>48</v>
@@ -4408,10 +4225,10 @@
     </row>
     <row r="120" spans="1:9" ht="19">
       <c r="A120" t="s">
-        <v>191</v>
+        <v>135</v>
       </c>
       <c r="B120" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C120" s="2">
         <v>4.57</v>
@@ -4419,8 +4236,8 @@
       <c r="D120" s="2">
         <v>1.29</v>
       </c>
-      <c r="E120" s="2" t="s">
-        <v>188</v>
+      <c r="E120" s="2">
+        <v>21.6</v>
       </c>
       <c r="F120" s="2">
         <v>15</v>
@@ -4434,10 +4251,10 @@
     </row>
     <row r="121" spans="1:9" ht="19">
       <c r="A121" t="s">
-        <v>192</v>
+        <v>136</v>
       </c>
       <c r="B121" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C121" s="2">
         <v>9</v>
@@ -4461,10 +4278,10 @@
     </row>
     <row r="122" spans="1:9" ht="19">
       <c r="A122" t="s">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="B122" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C122" s="2">
         <v>4.8600000000000003</v>
@@ -4487,10 +4304,10 @@
     </row>
     <row r="123" spans="1:9" ht="19">
       <c r="A123" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="B123" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C123" s="2">
         <v>3.11</v>
@@ -4498,8 +4315,8 @@
       <c r="D123" s="2">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E123" s="2" t="s">
-        <v>195</v>
+      <c r="E123" s="2">
+        <v>37.6</v>
       </c>
       <c r="F123" s="2">
         <v>47</v>
@@ -4513,10 +4330,10 @@
     </row>
     <row r="124" spans="1:9" ht="19">
       <c r="A124" t="s">
-        <v>196</v>
+        <v>139</v>
       </c>
       <c r="B124" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C124" s="2">
         <v>7.94</v>
@@ -4524,8 +4341,8 @@
       <c r="D124" s="2">
         <v>2.21</v>
       </c>
-      <c r="E124" s="2" t="s">
-        <v>197</v>
+      <c r="E124" s="2">
+        <v>11.3</v>
       </c>
       <c r="F124" s="2">
         <v>8</v>
@@ -4539,10 +4356,10 @@
     </row>
     <row r="125" spans="1:9" ht="19">
       <c r="A125" t="s">
-        <v>198</v>
+        <v>140</v>
       </c>
       <c r="B125" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C125" s="2">
         <v>5.68</v>
@@ -4550,8 +4367,8 @@
       <c r="D125" s="2">
         <v>1.74</v>
       </c>
-      <c r="E125" s="2" t="s">
-        <v>199</v>
+      <c r="E125" s="2">
+        <v>6.3</v>
       </c>
       <c r="F125" s="2">
         <v>5</v>
@@ -4565,10 +4382,10 @@
     </row>
     <row r="126" spans="1:9" ht="19">
       <c r="A126" t="s">
-        <v>200</v>
+        <v>141</v>
       </c>
       <c r="B126" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C126" s="2">
         <v>3.75</v>
@@ -4592,10 +4409,10 @@
     </row>
     <row r="127" spans="1:9" ht="19">
       <c r="A127" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="B127" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C127" s="2">
         <v>3.51</v>
@@ -4603,8 +4420,8 @@
       <c r="D127" s="2">
         <v>1.03</v>
       </c>
-      <c r="E127" s="2" t="s">
-        <v>202</v>
+      <c r="E127" s="2">
+        <v>89.6</v>
       </c>
       <c r="F127" s="2">
         <v>84</v>
@@ -4618,10 +4435,10 @@
     </row>
     <row r="128" spans="1:9" ht="19">
       <c r="A128" t="s">
-        <v>203</v>
+        <v>143</v>
       </c>
       <c r="B128" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C128" s="2">
         <v>3.24</v>
@@ -4629,8 +4446,8 @@
       <c r="D128" s="2">
         <v>1.17</v>
       </c>
-      <c r="E128" s="2" t="s">
-        <v>204</v>
+      <c r="E128" s="2">
+        <v>33.299999999999997</v>
       </c>
       <c r="F128" s="2">
         <v>33</v>
@@ -4644,10 +4461,10 @@
     </row>
     <row r="129" spans="1:8" ht="19">
       <c r="A129" t="s">
-        <v>205</v>
+        <v>144</v>
       </c>
       <c r="B129" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C129" s="2">
         <v>5.63</v>
@@ -4670,10 +4487,10 @@
     </row>
     <row r="130" spans="1:8" ht="19">
       <c r="A130" t="s">
-        <v>206</v>
+        <v>145</v>
       </c>
       <c r="B130" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
       <c r="C130" s="2">
         <v>2.3199999999999998</v>

</xml_diff>